<commit_message>
Optimizasyon kısmına kadarki modüllerin nihai halinin verilmesi.
</commit_message>
<xml_diff>
--- a/src/Presentation/Nop.Web/App_Data/FacultyExcellImport.xlsx
+++ b/src/Presentation/Nop.Web/App_Data/FacultyExcellImport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmert/BAU/Optimization-Web-App/Optimization-Web-App/src/Presentation/Nop.Web/App_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3ECD9115-9261-344D-9755-72A46A5C397F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179C1557-76AD-B14C-9841-22AA224EFBFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45540" yWindow="4480" windowWidth="32320" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Faculty" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -29,95 +29,53 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Faculty of Dentistry</t>
-  </si>
-  <si>
-    <t>Faculty of Pharmacy</t>
-  </si>
-  <si>
-    <t>Faculty of Education Sciences</t>
-  </si>
-  <si>
-    <t>Faculty of Law</t>
-  </si>
-  <si>
-    <t>Faculty of Communication</t>
-  </si>
-  <si>
-    <t>Faculty of Economics, Administration, and Social Sciences</t>
-  </si>
-  <si>
-    <t>Conservatory</t>
-  </si>
-  <si>
-    <t>Faculty of Architecture and Design</t>
-  </si>
-  <si>
-    <t>Faculty of Engineering and Natural Sciences</t>
-  </si>
-  <si>
-    <t>Faculty of Health Sciences</t>
-  </si>
-  <si>
-    <t>Faculty of Medicine</t>
-  </si>
-  <si>
-    <t>School of Health Services</t>
-  </si>
-  <si>
-    <t>Department of Gastronomy and Culinary Arts</t>
-  </si>
-  <si>
-    <t>Department of Aviation</t>
-  </si>
-  <si>
-    <t>Provides education and training in the field of dentistry.</t>
-  </si>
-  <si>
-    <t>Focuses on the study and practice of pharmaceutical sciences.</t>
-  </si>
-  <si>
-    <t>Prepares individuals for careers in the field of education.</t>
-  </si>
-  <si>
-    <t>Offers legal education and training for future legal professionals.</t>
-  </si>
-  <si>
-    <t>Covers various aspects of communication, including media and journalism.</t>
-  </si>
-  <si>
-    <t>Focuses on economics, administration, and social sciences.</t>
-  </si>
-  <si>
-    <t>Offers education in performing arts such as music, dance, and theater.</t>
-  </si>
-  <si>
-    <t>Provides education and training in architecture and design fields.</t>
-  </si>
-  <si>
-    <t>Focuses on engineering and natural sciences disciplines.</t>
-  </si>
-  <si>
-    <t>Offers programs in various health-related disciplines.</t>
-  </si>
-  <si>
-    <t>Provides medical education and training for future doctors.</t>
-  </si>
-  <si>
-    <t>Offers vocational training in health services.</t>
-  </si>
-  <si>
-    <t>Focuses on the study and practice of gastronomy and culinary arts.</t>
-  </si>
-  <si>
-    <t>Provides education and training for aspiring pilots.</t>
+    <t>ECZACILIK FAKÜLTESİ</t>
+  </si>
+  <si>
+    <t>EĞİTİM BİLİMLERİ FAKÜLTESİ</t>
+  </si>
+  <si>
+    <t>HUKUK FAKÜLTESİ</t>
+  </si>
+  <si>
+    <t>İKTİSADİ, İDARİ VE SOSYAL BİLİMLER FAKÜLTESİ</t>
+  </si>
+  <si>
+    <t>İLETİŞİM FAKÜLTESİ</t>
+  </si>
+  <si>
+    <t>MÜHENDİSLİK VE DOĞA BİLİMLERİ FAKÜLTESİ</t>
+  </si>
+  <si>
+    <t>UYGULAMALI BİLİMLER YÜKSEKOKULU</t>
+  </si>
+  <si>
+    <t>Faculty dedicated to the study of law, providing education and training to future legal professionals.</t>
+  </si>
+  <si>
+    <t>Faculty that specializes in the study of communication, providing comprehensive education and practical skills in various aspects of media, journalism, public relations, and related fields.</t>
+  </si>
+  <si>
+    <t>Faculty focused on the fields of economics, administration, and social sciences, offering comprehensive education and research opportunities in these disciplines.</t>
+  </si>
+  <si>
+    <t>Faculty dedicated to engineering and natural sciences, offering comprehensive education and research opportunities in fields such as physics, chemistry, mathematics, and various branches of engineering.</t>
+  </si>
+  <si>
+    <t>Higher education institution focused on applied sciences, providing practical-oriented education and training in fields such as technology, computer science, healthcare, and other vocational disciplines.</t>
+  </si>
+  <si>
+    <t>Faculty dedicated to the study of pharmacy, offering comprehensive education and training to future pharmacists, equipping them with knowledge and skills in pharmaceutical sciences, patient care, and medication management.</t>
+  </si>
+  <si>
+    <t>Faculty specializing in the field of education, providing comprehensive education and research opportunities for future educators, administrators, and researchers, with a focus on pedagogy, curriculum development, and educational psychology.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -130,6 +88,17 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
     </font>
   </fonts>
   <fills count="3">
@@ -157,11 +126,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -465,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -486,115 +461,59 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
         <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>